<commit_message>
updated exp script and images
</commit_message>
<xml_diff>
--- a/html/resources/trialorder/3_priming_recognition_test.xlsx
+++ b/html/resources/trialorder/3_priming_recognition_test.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandradecker/Dropbox/Projects/reactivate/trialorder/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761A9A02-7F06-3E4A-9D2B-0F2F9A0C618D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-27080" yWindow="840" windowWidth="18000" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -640,8 +646,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,6 +710,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -750,7 +764,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -782,9 +796,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -816,6 +848,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -991,14 +1041,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1087,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1049,7 +1104,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1121,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1083,7 +1138,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1100,7 +1155,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1117,7 +1172,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1134,7 +1189,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1151,7 +1206,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1168,7 +1223,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1185,7 +1240,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1202,7 +1257,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1274,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1236,7 +1291,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1253,7 +1308,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1270,7 +1325,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1287,7 +1342,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1304,7 +1359,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1321,7 +1376,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1338,7 +1393,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1355,7 +1410,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1372,7 +1427,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1389,7 +1444,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1406,7 +1461,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1423,7 +1478,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1440,7 +1495,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1457,7 +1512,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1474,7 +1529,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1491,7 +1546,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1508,7 +1563,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1525,7 +1580,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1542,7 +1597,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1559,7 +1614,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1576,7 +1631,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1593,7 +1648,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1610,7 +1665,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1627,7 +1682,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1644,7 +1699,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1661,7 +1716,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1678,7 +1733,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1695,7 +1750,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1712,7 +1767,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1729,7 +1784,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1746,7 +1801,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1763,7 +1818,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1780,7 +1835,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1797,7 +1852,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1814,7 +1869,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1831,7 +1886,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1848,7 +1903,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1865,7 +1920,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1882,7 +1937,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1899,7 +1954,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1916,7 +1971,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1933,7 +1988,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -1950,7 +2005,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -1967,7 +2022,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -1984,7 +2039,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -2001,7 +2056,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -2018,7 +2073,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -2035,7 +2090,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -2052,7 +2107,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -2069,7 +2124,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -2086,7 +2141,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -2103,7 +2158,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -2120,7 +2175,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -2137,7 +2192,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2154,7 +2209,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2171,7 +2226,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -2188,7 +2243,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -2205,7 +2260,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -2222,7 +2277,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -2239,7 +2294,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2256,7 +2311,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -2273,7 +2328,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -2290,7 +2345,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2307,7 +2362,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -2324,7 +2379,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2341,7 +2396,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -2358,7 +2413,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>84</v>
       </c>
@@ -2375,7 +2430,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -2392,7 +2447,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -2409,7 +2464,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -2426,7 +2481,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -2443,7 +2498,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -2460,7 +2515,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -2477,7 +2532,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -2494,7 +2549,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -2511,7 +2566,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -2528,7 +2583,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -2545,7 +2600,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2562,7 +2617,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -2579,7 +2634,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -2596,7 +2651,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -2613,7 +2668,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -2630,7 +2685,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -2647,7 +2702,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -2664,7 +2719,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -2681,7 +2736,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -2698,7 +2753,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>104</v>
       </c>
@@ -2715,7 +2770,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -2732,7 +2787,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -2749,7 +2804,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -2766,7 +2821,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -2783,7 +2838,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>109</v>
       </c>
@@ -2800,7 +2855,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -2817,7 +2872,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -2834,7 +2889,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>112</v>
       </c>
@@ -2851,7 +2906,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>113</v>
       </c>
@@ -2868,7 +2923,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>114</v>
       </c>
@@ -2885,7 +2940,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -2902,7 +2957,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>116</v>
       </c>
@@ -2919,7 +2974,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>117</v>
       </c>
@@ -2936,7 +2991,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>118</v>
       </c>
@@ -2953,7 +3008,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -2970,7 +3025,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -2987,7 +3042,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>121</v>
       </c>
@@ -3004,7 +3059,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>122</v>
       </c>
@@ -3021,7 +3076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>123</v>
       </c>
@@ -3038,7 +3093,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -3055,7 +3110,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>125</v>
       </c>
@@ -3072,7 +3127,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>126</v>
       </c>
@@ -3089,7 +3144,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>127</v>
       </c>
@@ -3106,7 +3161,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>128</v>
       </c>
@@ -3123,7 +3178,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>129</v>
       </c>
@@ -3140,7 +3195,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>130</v>
       </c>
@@ -3157,7 +3212,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>131</v>
       </c>
@@ -3174,7 +3229,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>132</v>
       </c>
@@ -3191,7 +3246,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>133</v>
       </c>
@@ -3208,7 +3263,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>134</v>
       </c>
@@ -3225,7 +3280,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>135</v>
       </c>
@@ -3242,7 +3297,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>136</v>
       </c>
@@ -3259,7 +3314,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>137</v>
       </c>
@@ -3276,7 +3331,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>138</v>
       </c>
@@ -3293,7 +3348,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>139</v>
       </c>
@@ -3310,7 +3365,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>140</v>
       </c>
@@ -3327,7 +3382,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>141</v>
       </c>
@@ -3344,7 +3399,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>142</v>
       </c>
@@ -3361,7 +3416,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>143</v>
       </c>
@@ -3378,7 +3433,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>144</v>
       </c>
@@ -3395,7 +3450,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>145</v>
       </c>
@@ -3412,7 +3467,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>146</v>
       </c>
@@ -3429,7 +3484,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>147</v>
       </c>
@@ -3446,7 +3501,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>148</v>
       </c>
@@ -3463,7 +3518,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>149</v>
       </c>
@@ -3480,7 +3535,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>150</v>
       </c>
@@ -3497,7 +3552,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>151</v>
       </c>
@@ -3514,7 +3569,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>152</v>
       </c>
@@ -3531,7 +3586,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -3548,7 +3603,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>154</v>
       </c>
@@ -3565,7 +3620,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>155</v>
       </c>
@@ -3582,7 +3637,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>156</v>
       </c>
@@ -3599,7 +3654,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>157</v>
       </c>
@@ -3616,7 +3671,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>158</v>
       </c>
@@ -3633,7 +3688,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>159</v>
       </c>
@@ -3650,7 +3705,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>160</v>
       </c>
@@ -3667,7 +3722,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>161</v>
       </c>
@@ -3684,7 +3739,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>162</v>
       </c>
@@ -3701,7 +3756,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>163</v>
       </c>
@@ -3718,7 +3773,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>164</v>
       </c>
@@ -3735,7 +3790,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>165</v>
       </c>
@@ -3752,7 +3807,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>166</v>
       </c>
@@ -3769,7 +3824,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>167</v>
       </c>
@@ -3786,7 +3841,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>168</v>
       </c>
@@ -3803,7 +3858,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>169</v>
       </c>
@@ -3820,7 +3875,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>170</v>
       </c>
@@ -3837,7 +3892,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>171</v>
       </c>
@@ -3854,7 +3909,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>172</v>
       </c>
@@ -3871,7 +3926,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>173</v>
       </c>
@@ -3888,7 +3943,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>174</v>
       </c>
@@ -3905,7 +3960,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>175</v>
       </c>
@@ -3922,7 +3977,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>176</v>
       </c>
@@ -3939,7 +3994,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>177</v>
       </c>
@@ -3956,7 +4011,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>178</v>
       </c>
@@ -3973,7 +4028,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>179</v>
       </c>
@@ -3990,7 +4045,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>180</v>
       </c>
@@ -4007,7 +4062,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>181</v>
       </c>
@@ -4024,7 +4079,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>182</v>
       </c>
@@ -4041,7 +4096,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>183</v>
       </c>
@@ -4058,7 +4113,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>184</v>
       </c>
@@ -4075,7 +4130,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>185</v>
       </c>
@@ -4092,7 +4147,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>186</v>
       </c>
@@ -4109,7 +4164,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>187</v>
       </c>
@@ -4126,7 +4181,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>188</v>
       </c>
@@ -4143,7 +4198,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>189</v>
       </c>
@@ -4160,7 +4215,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>190</v>
       </c>
@@ -4177,7 +4232,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>191</v>
       </c>
@@ -4194,7 +4249,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>192</v>
       </c>
@@ -4211,7 +4266,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>193</v>
       </c>
@@ -4228,7 +4283,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>194</v>
       </c>
@@ -4245,7 +4300,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>195</v>
       </c>
@@ -4262,7 +4317,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>196</v>
       </c>

</xml_diff>